<commit_message>
Atmos 22 code now working
</commit_message>
<xml_diff>
--- a/Hardware Information/Pin List.xlsx
+++ b/Hardware Information/Pin List.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nipun/Documents/Arduino/LEMSv2/Hardware Information/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{8715C3FC-2C71-0C4B-A68B-ECA5279B0650}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-33280" yWindow="1960" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin List" sheetId="1" r:id="rId1"/>
     <sheet name="Screw Terminals" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -162,12 +163,6 @@
     <t>Note: 3.3V/Ground connections not shown unless necessary</t>
   </si>
   <si>
-    <t>Upper 5TM Data</t>
-  </si>
-  <si>
-    <t>Lower 5TM Data</t>
-  </si>
-  <si>
     <t>Green LED</t>
   </si>
   <si>
@@ -189,12 +184,6 @@
     <t>Davis Wind Speed</t>
   </si>
   <si>
-    <t>Upper 5TM Power</t>
-  </si>
-  <si>
-    <t>Lower 5TM Power</t>
-  </si>
-  <si>
     <t>On-board Blue LED</t>
   </si>
   <si>
@@ -373,12 +362,24 @@
   </si>
   <si>
     <t>Fan Pin</t>
+  </si>
+  <si>
+    <t>Upper 5TM Data/Upper Teros21 Data</t>
+  </si>
+  <si>
+    <t>Lower 5TM Power/Lower Teros21 Power</t>
+  </si>
+  <si>
+    <t>Upper 5TM Power/Upper Teros21 Power</t>
+  </si>
+  <si>
+    <t>Lower 5TM Data/Lower Teros21 Data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -442,6 +443,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -709,17 +713,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -740,10 +744,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -754,13 +758,13 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -774,7 +778,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -782,13 +786,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -799,7 +803,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -807,13 +811,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -821,13 +825,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -835,13 +839,13 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -849,13 +853,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -863,13 +867,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -877,13 +881,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -891,13 +895,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -908,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -919,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -927,13 +931,13 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -944,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -952,13 +956,13 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -966,13 +970,13 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -980,13 +984,13 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1011,13 +1015,13 @@
         <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1028,7 +1032,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1039,7 +1043,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1050,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1061,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1072,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1080,13 +1084,13 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1100,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1111,7 +1115,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1122,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1133,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1141,13 +1145,13 @@
         <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1155,13 +1159,13 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1169,13 +1173,13 @@
         <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1183,13 +1187,13 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1197,13 +1201,13 @@
         <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1222,7 +1226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1240,24 +1244,24 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1266,28 +1270,28 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1296,15 +1300,15 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1313,15 +1317,15 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1330,15 +1334,15 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -1347,15 +1351,15 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1364,15 +1368,15 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1381,28 +1385,28 @@
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -1411,28 +1415,28 @@
         <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>3</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1441,15 +1445,15 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B15">
         <v>2</v>
@@ -1458,15 +1462,15 @@
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1475,15 +1479,15 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>4</v>
@@ -1492,15 +1496,15 @@
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B18">
         <f>SUM(B3:B17)</f>

</xml_diff>